<commit_message>
update pada send email
</commit_message>
<xml_diff>
--- a/Menu Tender.xlsx
+++ b/Menu Tender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/Project/tender-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\example-apps\tender-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD066B6E-5C7C-DE40-9C20-BFAEA134C171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343F37A6-2AD7-4D0A-B4B4-BDBE7F2245FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="13880" activeTab="1" xr2:uid="{4A00EBD2-0809-7C46-AF54-B8EB877996D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{4A00EBD2-0809-7C46-AF54-B8EB877996D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>Role</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>noKtp</t>
+  </si>
+  <si>
+    <t>remark</t>
   </si>
 </sst>
 </file>
@@ -577,13 +580,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -594,7 +597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -608,7 +611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>6</v>
       </c>
@@ -616,7 +619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>7</v>
       </c>
@@ -624,12 +627,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -640,7 +643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>6</v>
       </c>
@@ -648,7 +651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>7</v>
       </c>
@@ -656,12 +659,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>10</v>
       </c>
@@ -669,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>7</v>
       </c>
@@ -684,27 +687,27 @@
   <dimension ref="B3:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="2.83203125" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.875" customWidth="1"/>
+    <col min="5" max="5" width="2.625" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.83203125" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.875" customWidth="1"/>
+    <col min="12" max="12" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.625" customWidth="1"/>
+    <col min="14" max="14" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.625" customWidth="1"/>
+    <col min="16" max="16" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -730,7 +733,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -756,7 +759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -782,7 +785,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -808,7 +811,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -834,7 +837,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -857,7 +860,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
@@ -874,7 +880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>59</v>
       </c>
@@ -885,7 +891,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>33</v>
       </c>
@@ -893,7 +899,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>25</v>
       </c>
@@ -901,7 +907,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>18</v>
       </c>
@@ -909,7 +915,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>60</v>
       </c>
@@ -917,7 +923,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Update untuk create step klasifikasi
</commit_message>
<xml_diff>
--- a/Menu Tender.xlsx
+++ b/Menu Tender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\example-apps\tender-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/Project/tender-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343F37A6-2AD7-4D0A-B4B4-BDBE7F2245FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFEFD2E-D817-A34F-83A9-0846C2E4425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{4A00EBD2-0809-7C46-AF54-B8EB877996D5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{4A00EBD2-0809-7C46-AF54-B8EB877996D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -580,13 +580,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -597,7 +597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -611,7 +611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>6</v>
       </c>
@@ -619,7 +619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>7</v>
       </c>
@@ -627,12 +627,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -643,7 +643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>6</v>
       </c>
@@ -651,7 +651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>7</v>
       </c>
@@ -659,12 +659,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>10</v>
       </c>
@@ -672,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>7</v>
       </c>
@@ -690,24 +690,24 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="2.875" customWidth="1"/>
-    <col min="5" max="5" width="2.625" customWidth="1"/>
-    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" customWidth="1"/>
+    <col min="5" max="5" width="2.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="10" max="10" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.875" customWidth="1"/>
-    <col min="12" max="12" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.625" customWidth="1"/>
-    <col min="14" max="14" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.625" customWidth="1"/>
-    <col min="16" max="16" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -733,7 +733,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -759,7 +759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -785,7 +785,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -811,7 +811,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -837,7 +837,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -860,7 +860,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>62</v>
       </c>
@@ -880,7 +880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>59</v>
       </c>
@@ -891,7 +891,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
         <v>33</v>
       </c>
@@ -899,7 +899,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
         <v>25</v>
       </c>
@@ -907,7 +907,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>18</v>
       </c>
@@ -915,7 +915,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>60</v>
       </c>
@@ -923,7 +923,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="F15" t="s">
         <v>61</v>
       </c>

</xml_diff>